<commit_message>
IVP VP export updated
</commit_message>
<xml_diff>
--- a/storage/app/excel/templates/ivp-vp.xlsx
+++ b/storage/app/excel/templates/ivp-vp.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\business-processes\storage\app\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3DFB98-9A23-4B37-8786-29BA0548103D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F1D088-08F7-4282-8605-EE38F3F5974B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F2A26C44-2D1F-413C-A575-90AC71DB4886}"/>
   </bookViews>
   <sheets>
-    <sheet name="List 1" sheetId="2" r:id="rId1"/>
+    <sheet name="List" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'List 1'!$A$3:$X$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$A$3:$AM$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+  <si>
+    <t>REGISTERING COUNTRIES</t>
+  </si>
+  <si>
+    <t>YES/NO</t>
+  </si>
+  <si>
+    <t>FORECAST ESTIMATES</t>
+  </si>
   <si>
     <t>#</t>
   </si>
@@ -54,6 +63,39 @@
     <t>SHELF LIFE</t>
   </si>
   <si>
+    <t>KZ</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>UZ</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
     <t>ZONE 4B</t>
   </si>
   <si>
@@ -67,6 +109,42 @@
   </si>
   <si>
     <t xml:space="preserve"> YEAR 3</t>
+  </si>
+  <si>
+    <t>Note: Please provide required info for highlighted cells.</t>
+  </si>
+  <si>
+    <t>Selected countries</t>
+  </si>
+  <si>
+    <t>KAZAKHSTAN</t>
+  </si>
+  <si>
+    <t>TURKMENISTAN</t>
+  </si>
+  <si>
+    <t>TAJIKISTAN</t>
+  </si>
+  <si>
+    <t>UZBEKISTAN</t>
+  </si>
+  <si>
+    <t>KYRGYZSTAN</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
+    <t>MONGOLIA</t>
+  </si>
+  <si>
+    <t>RUSSIA</t>
+  </si>
+  <si>
+    <t>ARMENIA</t>
+  </si>
+  <si>
+    <t>CAMBODIA</t>
   </si>
   <si>
     <t>Year Cr/Be</t>
@@ -89,13 +167,40 @@
   </si>
   <si>
     <t>COMM</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>KE</t>
+  </si>
+  <si>
+    <t>AZERBAIJAN</t>
+  </si>
+  <si>
+    <t>ALBANIA</t>
+  </si>
+  <si>
+    <t>KENYA</t>
+  </si>
+  <si>
+    <t>DOMINICAN REPUBLIC</t>
+  </si>
+  <si>
+    <t>BURMA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +244,15 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri Light"/>
       <family val="2"/>
@@ -148,6 +262,31 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="204"/>
@@ -162,13 +301,42 @@
       <charset val="204"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -188,8 +356,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -212,44 +392,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -257,7 +578,14 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="2" xr:uid="{CD7EB858-8418-49C0-9F23-2BD55089D5EE}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -575,217 +903,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB251C2F-0DEB-447E-982C-891A3EAD04FA}">
-  <dimension ref="A2:CA37"/>
+  <dimension ref="A1:AM24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="84.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11" style="10" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="14" style="10" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="10" customWidth="1"/>
-    <col min="7" max="9" width="15.42578125" style="10" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="10"/>
-    <col min="12" max="15" width="14" style="10" customWidth="1"/>
-    <col min="16" max="79" width="9.140625" style="10"/>
-    <col min="80" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="84.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="14" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="5" customWidth="1"/>
+    <col min="7" max="9" width="15.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="4.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="4.140625" style="5" customWidth="1"/>
+    <col min="23" max="23" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.140625" style="5"/>
+    <col min="27" max="30" width="14" style="5" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="47"/>
+    </row>
+    <row r="2" spans="1:39" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="S2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AM3" s="25"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="25"/>
+      <c r="AL4" s="25"/>
+      <c r="AM4" s="25"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="31"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="29"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="B16" s="37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="11"/>
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
-      <c r="D36" s="10"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
-      <c r="D37" s="10"/>
+      <c r="B17" s="37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:X3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="H10:I13 H15:I37 F14:I14">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="between">
+  <autoFilter ref="A3:AM3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="4">
+    <mergeCell ref="J1:X1"/>
+    <mergeCell ref="AE1:AG1"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="AK1:AM1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="J1:X1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>1</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:A24">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>1</formula>
       <formula>1</formula>
     </cfRule>

</xml_diff>